<commit_message>
Adding UI test scenarios
Checking the labels , controls, buttons etc present on the login page
</commit_message>
<xml_diff>
--- a/LoginPage_FB.xlsx
+++ b/LoginPage_FB.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>Project Name</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>Login Page</t>
+  </si>
+  <si>
+    <t>UI Tests</t>
   </si>
 </sst>
 </file>
@@ -223,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -259,11 +262,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -291,6 +320,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -569,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N43"/>
+  <dimension ref="A2:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -877,8 +912,10 @@
       <c r="N14" s="2"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="11"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1308,39 +1345,10 @@
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A15:B15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>